<commit_message>
Update Leave Card 8/4/2023 3:52 PM
</commit_message>
<xml_diff>
--- a/SHARED FOLDER/LEAVE CERTIFICATION/LEAVE CERTIFICATION DATA BANK.xlsx
+++ b/SHARED FOLDER/LEAVE CERTIFICATION/LEAVE CERTIFICATION DATA BANK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\SHARED FOLDER\LEAVE CERTIFICATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CFDF6B-9174-47B8-BA20-4A2BD4C8F35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912CC80-1B5A-436D-BEB3-2871E596F31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="329">
   <si>
     <t>NO</t>
   </si>
@@ -982,6 +982,57 @@
   </si>
   <si>
     <t>Office of the City Engineer(Parks &amp; Plaza Div) detailed at Picnic Grove</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TERESITA</t>
+  </si>
+  <si>
+    <t>ABAJETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HANNABELLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ARNOLD DEEJAY</t>
+  </si>
+  <si>
+    <t>EBARDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IVY</t>
+  </si>
+  <si>
+    <t>MARGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RUBEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RENE ROSE</t>
+  </si>
+  <si>
+    <r>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ñ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -992,7 +1043,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,6 +1064,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1035,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1062,6 +1119,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1144,8 +1229,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U85" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:U85" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U89" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:U89" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U73">
     <sortCondition ref="A1:A73"/>
   </sortState>
@@ -1479,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U85"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N66" workbookViewId="0">
-      <selection activeCell="S86" sqref="S86"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6846,7 +6931,7 @@
         <v>45112</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>274</v>
+        <v>28</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>21</v>
@@ -6908,70 +6993,414 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="str">
+      <c r="A84" s="2">
         <f>IF(ISBLANK(Table1[[#This Row],[DATE CREATED]]),"",A83+1)</f>
-        <v/>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="B84" s="4">
+        <v>45142</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="H84" s="1" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[LASTNAME]]),"------",CONCATENATE(Table1[[#This Row],[FIRSTNAME]]," ",IF(ISBLANK(Table1[[#This Row],[MIDDLE INITIAL]]),"",LEFT(Table1[[#This Row],[MIDDLE INITIAL]],1)&amp;". "),Table1[[#This Row],[LASTNAME]]))</f>
-        <v>------</v>
-      </c>
-      <c r="K84" s="8"/>
-      <c r="L84" s="8"/>
-      <c r="M84" s="8" t="str">
+        <v xml:space="preserve"> TERESITA P. RIÑO</v>
+      </c>
+      <c r="I84" t="s">
+        <v>208</v>
+      </c>
+      <c r="J84" t="s">
+        <v>260</v>
+      </c>
+      <c r="K84" s="8">
+        <v>42552</v>
+      </c>
+      <c r="L84" s="8">
+        <v>44742</v>
+      </c>
+      <c r="M84" s="8">
         <f>IF(ISBLANK(Table1[[#This Row],[LASTDAY OF SERVICE]]),"---",Table1[[#This Row],[LASTDAY OF SERVICE]]+1)</f>
-        <v>---</v>
-      </c>
-      <c r="N84" s="5"/>
-      <c r="O84" s="7"/>
-      <c r="P84" s="7"/>
+        <v>44743</v>
+      </c>
+      <c r="N84" s="5">
+        <v>11814</v>
+      </c>
+      <c r="O84" s="7">
+        <v>47.5</v>
+      </c>
+      <c r="P84" s="7">
+        <v>67.5</v>
+      </c>
       <c r="Q84" s="7">
         <f>SUM(Table1[[#This Row],[VACATION LEAVE]:[SICK LEAVE]])</f>
-        <v>0</v>
-      </c>
-      <c r="S84" s="6" t="str">
+        <v>115</v>
+      </c>
+      <c r="R84" s="1">
+        <v>4.8192699999999998E-2</v>
+      </c>
+      <c r="S84" s="6">
         <f>IF(ISBLANK(Table1[[#This Row],[MONTHLY SALARY]]),"-------",PRODUCT(N84,Q84:R84))</f>
-        <v>-------</v>
+        <v>65475.084146999994</v>
+      </c>
+      <c r="T84" s="1" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="str">
+      <c r="A85" s="2">
         <f>IF(ISBLANK(Table1[[#This Row],[DATE CREATED]]),"",A84+1)</f>
-        <v/>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="B85" s="4">
+        <v>45142</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="H85" s="1" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[LASTNAME]]),"------",CONCATENATE(Table1[[#This Row],[FIRSTNAME]]," ",IF(ISBLANK(Table1[[#This Row],[MIDDLE INITIAL]]),"",LEFT(Table1[[#This Row],[MIDDLE INITIAL]],1)&amp;". "),Table1[[#This Row],[LASTNAME]]))</f>
-        <v>------</v>
-      </c>
-      <c r="K85" s="8"/>
-      <c r="L85" s="8"/>
-      <c r="M85" s="8" t="str">
+        <v xml:space="preserve"> HANNABELLE E. ABAJETO</v>
+      </c>
+      <c r="I85" t="s">
+        <v>208</v>
+      </c>
+      <c r="J85" t="s">
+        <v>260</v>
+      </c>
+      <c r="K85" s="8">
+        <v>42767</v>
+      </c>
+      <c r="L85" s="8">
+        <v>44742</v>
+      </c>
+      <c r="M85" s="8">
         <f>IF(ISBLANK(Table1[[#This Row],[LASTDAY OF SERVICE]]),"---",Table1[[#This Row],[LASTDAY OF SERVICE]]+1)</f>
-        <v>---</v>
-      </c>
-      <c r="N85" s="5"/>
-      <c r="O85" s="7"/>
-      <c r="P85" s="7"/>
+        <v>44743</v>
+      </c>
+      <c r="N85" s="5">
+        <v>11814</v>
+      </c>
+      <c r="O85" s="7">
+        <v>47.5</v>
+      </c>
+      <c r="P85" s="7">
+        <v>67.5</v>
+      </c>
       <c r="Q85" s="7">
         <f>SUM(Table1[[#This Row],[VACATION LEAVE]:[SICK LEAVE]])</f>
-        <v>0</v>
-      </c>
-      <c r="S85" s="6" t="str">
+        <v>115</v>
+      </c>
+      <c r="R85" s="1">
+        <v>4.8192699999999998E-2</v>
+      </c>
+      <c r="S85" s="6">
         <f>IF(ISBLANK(Table1[[#This Row],[MONTHLY SALARY]]),"-------",PRODUCT(N85,Q85:R85))</f>
-        <v>-------</v>
+        <v>65475.084146999994</v>
+      </c>
+      <c r="T85" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="11">
+        <f>IF(ISBLANK(Table1[[#This Row],[DATE CREATED]]),"",A85+1)</f>
+        <v>85</v>
+      </c>
+      <c r="B86" s="12">
+        <v>45142</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H86" s="14" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTNAME]]),"------",CONCATENATE(Table1[[#This Row],[FIRSTNAME]]," ",IF(ISBLANK(Table1[[#This Row],[MIDDLE INITIAL]]),"",LEFT(Table1[[#This Row],[MIDDLE INITIAL]],1)&amp;". "),Table1[[#This Row],[LASTNAME]]))</f>
+        <v xml:space="preserve"> ARNOLD DEEJAY S. DIMAPILIS</v>
+      </c>
+      <c r="I86" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="J86" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="K86" s="16">
+        <v>42552</v>
+      </c>
+      <c r="L86" s="16">
+        <v>44742</v>
+      </c>
+      <c r="M86" s="16">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTDAY OF SERVICE]]),"---",Table1[[#This Row],[LASTDAY OF SERVICE]]+1)</f>
+        <v>44743</v>
+      </c>
+      <c r="N86" s="17">
+        <v>11814</v>
+      </c>
+      <c r="O86" s="18">
+        <v>47.5</v>
+      </c>
+      <c r="P86" s="18">
+        <v>67.5</v>
+      </c>
+      <c r="Q86" s="18">
+        <f>SUM(Table1[[#This Row],[VACATION LEAVE]:[SICK LEAVE]])</f>
+        <v>115</v>
+      </c>
+      <c r="R86" s="13">
+        <v>4.8192699999999998E-2</v>
+      </c>
+      <c r="S86" s="19">
+        <f>IF(ISBLANK(Table1[[#This Row],[MONTHLY SALARY]]),"-------",PRODUCT(N86,Q86:R86))</f>
+        <v>65475.084146999994</v>
+      </c>
+      <c r="T86" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="11">
+        <f>IF(ISBLANK(Table1[[#This Row],[DATE CREATED]]),"",A86+1)</f>
+        <v>86</v>
+      </c>
+      <c r="B87" s="12">
+        <v>45142</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="G87" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H87" s="14" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTNAME]]),"------",CONCATENATE(Table1[[#This Row],[FIRSTNAME]]," ",IF(ISBLANK(Table1[[#This Row],[MIDDLE INITIAL]]),"",LEFT(Table1[[#This Row],[MIDDLE INITIAL]],1)&amp;". "),Table1[[#This Row],[LASTNAME]]))</f>
+        <v xml:space="preserve"> IVY B. EBARDO</v>
+      </c>
+      <c r="I87" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="J87" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="K87" s="16">
+        <v>42857</v>
+      </c>
+      <c r="L87" s="16">
+        <v>44742</v>
+      </c>
+      <c r="M87" s="16">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTDAY OF SERVICE]]),"---",Table1[[#This Row],[LASTDAY OF SERVICE]]+1)</f>
+        <v>44743</v>
+      </c>
+      <c r="N87" s="17">
+        <v>11814</v>
+      </c>
+      <c r="O87" s="18">
+        <v>47.5</v>
+      </c>
+      <c r="P87" s="18">
+        <v>67.5</v>
+      </c>
+      <c r="Q87" s="18">
+        <f>SUM(Table1[[#This Row],[VACATION LEAVE]:[SICK LEAVE]])</f>
+        <v>115</v>
+      </c>
+      <c r="R87" s="13">
+        <v>4.8192699999999998E-2</v>
+      </c>
+      <c r="S87" s="19">
+        <f>IF(ISBLANK(Table1[[#This Row],[MONTHLY SALARY]]),"-------",PRODUCT(N87,Q87:R87))</f>
+        <v>65475.084146999994</v>
+      </c>
+      <c r="T87" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="11">
+        <f>IF(ISBLANK(Table1[[#This Row],[DATE CREATED]]),"",A87+1)</f>
+        <v>87</v>
+      </c>
+      <c r="B88" s="12">
+        <v>45142</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="G88" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H88" s="14" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTNAME]]),"------",CONCATENATE(Table1[[#This Row],[FIRSTNAME]]," ",IF(ISBLANK(Table1[[#This Row],[MIDDLE INITIAL]]),"",LEFT(Table1[[#This Row],[MIDDLE INITIAL]],1)&amp;". "),Table1[[#This Row],[LASTNAME]]))</f>
+        <v xml:space="preserve"> RUBEN C. MARGES</v>
+      </c>
+      <c r="I88" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="J88" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="K88" s="16">
+        <v>42857</v>
+      </c>
+      <c r="L88" s="16">
+        <v>44742</v>
+      </c>
+      <c r="M88" s="16">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTDAY OF SERVICE]]),"---",Table1[[#This Row],[LASTDAY OF SERVICE]]+1)</f>
+        <v>44743</v>
+      </c>
+      <c r="N88" s="17">
+        <v>11814</v>
+      </c>
+      <c r="O88" s="18">
+        <v>47.5</v>
+      </c>
+      <c r="P88" s="18">
+        <v>67.5</v>
+      </c>
+      <c r="Q88" s="18">
+        <f>SUM(Table1[[#This Row],[VACATION LEAVE]:[SICK LEAVE]])</f>
+        <v>115</v>
+      </c>
+      <c r="R88" s="13">
+        <v>4.8192699999999998E-2</v>
+      </c>
+      <c r="S88" s="19">
+        <f>IF(ISBLANK(Table1[[#This Row],[MONTHLY SALARY]]),"-------",PRODUCT(N88,Q88:R88))</f>
+        <v>65475.084146999994</v>
+      </c>
+      <c r="T88" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <f>IF(ISBLANK(Table1[[#This Row],[DATE CREATED]]),"",A88+1)</f>
+        <v>88</v>
+      </c>
+      <c r="B89" s="4">
+        <v>45142</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H89" s="10" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTNAME]]),"------",CONCATENATE(Table1[[#This Row],[FIRSTNAME]]," ",IF(ISBLANK(Table1[[#This Row],[MIDDLE INITIAL]]),"",LEFT(Table1[[#This Row],[MIDDLE INITIAL]],1)&amp;". "),Table1[[#This Row],[LASTNAME]]))</f>
+        <v xml:space="preserve"> RENE ROSE C. MENDOZA</v>
+      </c>
+      <c r="I89" t="s">
+        <v>208</v>
+      </c>
+      <c r="J89" t="s">
+        <v>260</v>
+      </c>
+      <c r="K89" s="8">
+        <v>42552</v>
+      </c>
+      <c r="L89" s="8">
+        <v>44742</v>
+      </c>
+      <c r="M89" s="8">
+        <f>IF(ISBLANK(Table1[[#This Row],[LASTDAY OF SERVICE]]),"---",Table1[[#This Row],[LASTDAY OF SERVICE]]+1)</f>
+        <v>44743</v>
+      </c>
+      <c r="N89" s="5">
+        <v>11814</v>
+      </c>
+      <c r="O89" s="7">
+        <v>47.5</v>
+      </c>
+      <c r="P89" s="7">
+        <v>67.5</v>
+      </c>
+      <c r="Q89" s="7">
+        <f>SUM(Table1[[#This Row],[VACATION LEAVE]:[SICK LEAVE]])</f>
+        <v>115</v>
+      </c>
+      <c r="R89" s="1">
+        <v>4.8192699999999998E-2</v>
+      </c>
+      <c r="S89" s="6">
+        <f>IF(ISBLANK(Table1[[#This Row],[MONTHLY SALARY]]),"-------",PRODUCT(N89,Q89:R89))</f>
+        <v>65475.084146999994</v>
+      </c>
+      <c r="T89" s="1" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D85" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D89" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"MR, MS,MRS,DR,ATTY,ENGR, HON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C85" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C89" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"his, her"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>